<commit_message>
Included close_log function to clear memory msg_db and msg_log Modified init_msg_db so that it does not open multiple copies of the same message database
</commit_message>
<xml_diff>
--- a/samples/TestMsg_db.xlsx
+++ b/samples/TestMsg_db.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="TestMsg_db" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>short db message id 2,</t>
-  </si>
-  <si>
-    <t>short db message id -3,</t>
   </si>
   <si>
     <t>long db message id 1,</t>
@@ -877,7 +874,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -904,10 +901,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -918,24 +915,24 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>